<commit_message>
Lots of changes pre-meeting
</commit_message>
<xml_diff>
--- a/Data for Dashboard.xlsx
+++ b/Data for Dashboard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\devstuff\nodestuff\blur-admin-demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779A16A4-D549-415C-87A7-00F71A17A936}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA42F96-5521-4905-8692-57558DCE7FB1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="851" activeTab="9" xr2:uid="{9E5EBF5C-35EF-4D98-A641-A1750B1D59BE}"/>
+    <workbookView xWindow="4575" yWindow="3390" windowWidth="21600" windowHeight="11385" tabRatio="851" activeTab="4" xr2:uid="{9E5EBF5C-35EF-4D98-A641-A1750B1D59BE}"/>
   </bookViews>
   <sheets>
     <sheet name="HDR Students" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Staff Workforce" sheetId="9" r:id="rId8"/>
     <sheet name="Learning Teaching" sheetId="10" r:id="rId9"/>
     <sheet name="Budget" sheetId="11" r:id="rId10"/>
+    <sheet name="Enrolment" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>HDR Students</t>
   </si>
@@ -168,9 +169,6 @@
     <t>Underlying Operating Cash Flow ($mil)</t>
   </si>
   <si>
-    <t>Netcash ($mil)</t>
-  </si>
-  <si>
     <t>Financial</t>
   </si>
   <si>
@@ -226,6 +224,21 @@
   </si>
   <si>
     <t>Net Cash ($mil)</t>
+  </si>
+  <si>
+    <t>Enrolment</t>
+  </si>
+  <si>
+    <t>2012</t>
+  </si>
+  <si>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>Student Numbers</t>
   </si>
 </sst>
 </file>
@@ -388,66 +401,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF666666"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color rgb="FFDCDCDC"/>
-        </left>
-        <right style="medium">
-          <color rgb="FFDCDCDC"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF666666"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -785,6 +738,66 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF666666"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF666666"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color rgb="FFDCDCDC"/>
+        </left>
+        <right style="medium">
+          <color rgb="FFDCDCDC"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -1467,6 +1480,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -1486,6 +1504,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1505,6 +1528,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -1524,6 +1552,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -1543,6 +1576,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -1562,6 +1600,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1583,6 +1626,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -1604,6 +1652,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -1625,6 +1678,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -1646,6 +1704,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -1667,6 +1730,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -1688,6 +1756,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -1710,6 +1783,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-6B11-4FE0-8277-9D6823754FDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -4942,17 +5020,36 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{EF327501-572A-49B9-8849-EF7263EB4CF2}" name="BudgetTable" displayName="BudgetTable" ref="A1:H6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{EF327501-572A-49B9-8849-EF7263EB4CF2}" name="BudgetTable" displayName="BudgetTable" ref="A1:H6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:H6" xr:uid="{9C4EDFBD-0034-416C-A1C3-9ADEE355BAB9}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{FB885A2A-A091-4F37-926A-B949CDBEFEE6}" name="Column1" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{AEB425C8-D863-4FE8-98DD-847E269A7A97}" name="2014" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{1319E731-7838-484B-8954-73F67F88230D}" name="2015" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{57863488-6CB3-4C12-A595-849F19D34C90}" name="2016" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{2FEAF6F9-369A-4017-8C27-0DF3083F33FF}" name="2017" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{226AF3F2-7E10-4C68-AC84-9142EE156CC8}" name="2018" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{33F7DA71-E53B-4E1E-8E29-62B1289D7227}" name="2019" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{4785145C-C70C-440A-A9F3-44E475B4BA1C}" name="Budget 2019" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{FB885A2A-A091-4F37-926A-B949CDBEFEE6}" name="Column1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{AEB425C8-D863-4FE8-98DD-847E269A7A97}" name="2014" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1319E731-7838-484B-8954-73F67F88230D}" name="2015" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{57863488-6CB3-4C12-A595-849F19D34C90}" name="2016" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2FEAF6F9-369A-4017-8C27-0DF3083F33FF}" name="2017" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{226AF3F2-7E10-4C68-AC84-9142EE156CC8}" name="2018" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{33F7DA71-E53B-4E1E-8E29-62B1289D7227}" name="2019" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4785145C-C70C-440A-A9F3-44E475B4BA1C}" name="Budget 2019" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D004E21B-60DB-4359-9136-D91287A79C71}" name="EnrolmentTable" displayName="EnrolmentTable" ref="A2:J3" totalsRowShown="0">
+  <autoFilter ref="A2:J3" xr:uid="{E03A18A8-4555-4647-8EAA-E07AB7076BB3}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{077C6356-AF6E-4B20-BB26-AF00A6FD75D1}" name="Year"/>
+    <tableColumn id="2" xr3:uid="{5871544D-418F-44D6-B419-26A3B6FBFC67}" name="2012"/>
+    <tableColumn id="3" xr3:uid="{3EF36A36-8C1B-4299-96AC-9A9041D0EA20}" name="2013"/>
+    <tableColumn id="4" xr3:uid="{A8C3F037-3B2D-491D-BBC8-FE10686CF939}" name="2014"/>
+    <tableColumn id="5" xr3:uid="{B29695AD-13C8-4E87-A6FF-6B9485CDE1E3}" name="2015"/>
+    <tableColumn id="6" xr3:uid="{14731BEB-C2F4-4A49-B5B8-FEAC352025E6}" name="2016"/>
+    <tableColumn id="7" xr3:uid="{CC4CEBD7-A2DE-46B7-B2EF-0ABDB5DE80A7}" name="2017"/>
+    <tableColumn id="8" xr3:uid="{DF4EBE90-2ADD-4F1D-A46F-6047FB1D13CC}" name="2018"/>
+    <tableColumn id="9" xr3:uid="{D20EB106-38C0-44D9-B4D7-8EFAC9B18B63}" name="2019"/>
+    <tableColumn id="10" xr3:uid="{9E174F00-52D0-45CC-BB79-95FAFE5A2D40}" name="2020"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5027,9 +5124,9 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{815DD22F-5DE8-4A5B-90D5-19CF4DC10A6B}" name="FinancialKPITable" displayName="FinancialKPITable" ref="A13:H18" totalsRowShown="0">
-  <autoFilter ref="A13:H18" xr:uid="{58D34FBD-CFBF-4B73-8065-D1D8C833084E}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{815DD22F-5DE8-4A5B-90D5-19CF4DC10A6B}" name="FinancialKPITable" displayName="FinancialKPITable" ref="A13:G16" totalsRowShown="0">
+  <autoFilter ref="A13:G16" xr:uid="{58D34FBD-CFBF-4B73-8065-D1D8C833084E}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{6209E204-394E-42E4-A0B6-D0F6B38C26FD}" name="Label"/>
     <tableColumn id="2" xr3:uid="{E92E77AA-6DE6-4B21-87BC-72987F89DDC9}" name="2014"/>
     <tableColumn id="3" xr3:uid="{B73C67AB-004E-4A61-9AD0-32B1F64A750F}" name="2015"/>
@@ -5037,7 +5134,6 @@
     <tableColumn id="5" xr3:uid="{1381B7D9-979F-4969-A334-D067E801587F}" name="2017"/>
     <tableColumn id="6" xr3:uid="{A66BD7F5-F814-480A-A456-C9DB064CDBED}" name="2018"/>
     <tableColumn id="7" xr3:uid="{FA8EB99D-C80B-4A19-B1A0-A184B57B8D03}" name="2019"/>
-    <tableColumn id="8" xr3:uid="{2FBEBA54-C8A5-4E07-8372-E51657732958}" name="Budget 2019"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5354,7 +5450,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5426,8 +5522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96AD98FB-190E-467D-8CB7-8652E8DF36A2}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5444,16 +5540,16 @@
         <v>18</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>47</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>32</v>
@@ -5571,7 +5667,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" s="12">
         <v>17.2</v>
@@ -5604,12 +5700,99 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A7C10C-108F-4801-A4F6-F8C759FE12B5}">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3">
+        <v>2720</v>
+      </c>
+      <c r="C3">
+        <v>2922</v>
+      </c>
+      <c r="D3">
+        <v>3033</v>
+      </c>
+      <c r="E3">
+        <v>3224</v>
+      </c>
+      <c r="F3">
+        <v>3382</v>
+      </c>
+      <c r="G3">
+        <v>3462</v>
+      </c>
+      <c r="H3">
+        <v>3874</v>
+      </c>
+      <c r="I3">
+        <v>4113</v>
+      </c>
+      <c r="J3">
+        <v>3626</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{022B3645-1919-4B6A-A92F-D42B2CC5833D}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5681,7 +5864,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5855,7 +6038,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5926,24 +6109,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3272AB5C-2293-405D-AEEA-8FC8556B3134}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -5954,7 +6136,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -5965,7 +6147,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -5976,7 +6158,7 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -5987,7 +6169,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -5998,12 +6180,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -6014,7 +6196,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>81.2</v>
       </c>
@@ -6022,26 +6204,26 @@
         <v>84.6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
       <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>45</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
       </c>
       <c r="F13" t="s">
         <v>32</v>
@@ -6049,138 +6231,74 @@
       <c r="G13" t="s">
         <v>33</v>
       </c>
-      <c r="H13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="C14">
-        <v>3.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D14">
-        <v>3.2</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>3.3</v>
+        <v>1.2</v>
       </c>
       <c r="F14">
-        <v>3.3</v>
+        <v>1.6</v>
       </c>
       <c r="G14">
-        <v>3.4</v>
-      </c>
-      <c r="H14">
-        <v>35.6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B15">
         <v>0.8</v>
       </c>
       <c r="C15">
+        <v>1.2</v>
+      </c>
+      <c r="D15">
+        <v>1.3</v>
+      </c>
+      <c r="E15">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D15">
+      <c r="F15">
+        <v>1.2</v>
+      </c>
+      <c r="G15">
         <v>1</v>
       </c>
-      <c r="E15">
-        <v>1.2</v>
-      </c>
-      <c r="F15">
-        <v>1.6</v>
-      </c>
-      <c r="G15">
-        <v>1.5</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B16">
-        <v>0.8</v>
+        <v>2.1</v>
       </c>
       <c r="C16">
-        <v>1.2</v>
+        <v>2.4</v>
       </c>
       <c r="D16">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E16">
-        <v>1.1000000000000001</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F16">
-        <v>1.2</v>
+        <v>1.7</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17">
-        <v>2.1</v>
-      </c>
-      <c r="C17">
-        <v>2.4</v>
-      </c>
-      <c r="D17">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E17">
         <v>2.2000000000000002</v>
-      </c>
-      <c r="F17">
-        <v>1.7</v>
-      </c>
-      <c r="G17">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18">
-        <v>17.2</v>
-      </c>
-      <c r="C18">
-        <v>16</v>
-      </c>
-      <c r="D18">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
-      <c r="F18">
-        <v>14</v>
-      </c>
-      <c r="G18">
-        <v>15.1</v>
-      </c>
-      <c r="H18">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -6199,7 +6317,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6213,7 +6331,7 @@
         <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6362,7 +6480,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>10574</v>
@@ -6392,7 +6510,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6429,7 +6547,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -6466,7 +6584,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -6527,7 +6645,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -6535,7 +6653,7 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6580,15 +6698,15 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
         <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -6613,7 +6731,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6624,7 +6742,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -6632,10 +6750,10 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>